<commit_message>
modify the excel file
</commit_message>
<xml_diff>
--- a/Burst-Detection/压力数据.xlsx
+++ b/Burst-Detection/压力数据.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5850" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="6300" windowWidth="22260" windowHeight="12645" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="平滑降噪" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="130">
   <si>
     <t>压力变化阈值</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -438,10 +438,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>为平滑</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">   </t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -503,6 +499,14 @@
   </si>
   <si>
     <t>漏报率</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>不平滑</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                                                 </t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1025,7 +1029,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1175,37 +1179,21 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1217,14 +1205,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1507,8 +1514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:R63"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70:P72"/>
+    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1613,13 +1620,13 @@
       </c>
     </row>
     <row r="7" spans="1:18">
-      <c r="A7" s="80" t="s">
+      <c r="A7" s="81" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:18">
-      <c r="A8" s="80"/>
-      <c r="B8" s="79" t="s">
+      <c r="A8" s="81"/>
+      <c r="B8" s="82" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="4">
@@ -1666,8 +1673,8 @@
       </c>
     </row>
     <row r="9" spans="1:18">
-      <c r="A9" s="80"/>
-      <c r="B9" s="79"/>
+      <c r="A9" s="81"/>
+      <c r="B9" s="82"/>
       <c r="C9" s="4">
         <v>0.20622203695893401</v>
       </c>
@@ -1712,8 +1719,8 @@
       </c>
     </row>
     <row r="10" spans="1:18">
-      <c r="A10" s="80"/>
-      <c r="B10" s="79" t="s">
+      <c r="A10" s="81"/>
+      <c r="B10" s="82" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="4">
@@ -1760,8 +1767,8 @@
       </c>
     </row>
     <row r="11" spans="1:18">
-      <c r="A11" s="80"/>
-      <c r="B11" s="79"/>
+      <c r="A11" s="81"/>
+      <c r="B11" s="82"/>
       <c r="C11" s="4">
         <v>6.2105197897433698E-2</v>
       </c>
@@ -1809,8 +1816,8 @@
       </c>
     </row>
     <row r="12" spans="1:18">
-      <c r="A12" s="80"/>
-      <c r="B12" s="79" t="s">
+      <c r="A12" s="81"/>
+      <c r="B12" s="82" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="4">
@@ -1857,8 +1864,8 @@
       </c>
     </row>
     <row r="13" spans="1:18">
-      <c r="A13" s="80"/>
-      <c r="B13" s="79"/>
+      <c r="A13" s="81"/>
+      <c r="B13" s="82"/>
       <c r="C13">
         <v>2.7664742714910401E-2</v>
       </c>
@@ -1903,8 +1910,8 @@
       </c>
     </row>
     <row r="14" spans="1:18">
-      <c r="A14" s="80"/>
-      <c r="B14" s="79" t="s">
+      <c r="A14" s="81"/>
+      <c r="B14" s="82" t="s">
         <v>18</v>
       </c>
       <c r="C14">
@@ -1951,8 +1958,8 @@
       </c>
     </row>
     <row r="15" spans="1:18">
-      <c r="A15" s="80"/>
-      <c r="B15" s="79"/>
+      <c r="A15" s="81"/>
+      <c r="B15" s="82"/>
       <c r="C15">
         <v>1.8060443331874398E-2</v>
       </c>
@@ -1997,8 +2004,8 @@
       </c>
     </row>
     <row r="16" spans="1:18">
-      <c r="A16" s="80"/>
-      <c r="B16" s="79" t="s">
+      <c r="A16" s="81"/>
+      <c r="B16" s="82" t="s">
         <v>19</v>
       </c>
       <c r="C16">
@@ -2045,8 +2052,8 @@
       </c>
     </row>
     <row r="17" spans="1:16">
-      <c r="A17" s="80"/>
-      <c r="B17" s="79"/>
+      <c r="A17" s="81"/>
+      <c r="B17" s="82"/>
       <c r="C17">
         <v>1.13857990146845E-2</v>
       </c>
@@ -2091,10 +2098,10 @@
       </c>
     </row>
     <row r="19" spans="1:16">
-      <c r="A19" s="80" t="s">
+      <c r="A19" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="79" t="s">
+      <c r="B19" s="82" t="s">
         <v>16</v>
       </c>
       <c r="C19" s="6">
@@ -2141,8 +2148,8 @@
       </c>
     </row>
     <row r="20" spans="1:16">
-      <c r="A20" s="80"/>
-      <c r="B20" s="79"/>
+      <c r="A20" s="81"/>
+      <c r="B20" s="82"/>
       <c r="C20" s="6">
         <v>0.233333333333334</v>
       </c>
@@ -2187,8 +2194,8 @@
       </c>
     </row>
     <row r="21" spans="1:16">
-      <c r="A21" s="80"/>
-      <c r="B21" s="79" t="s">
+      <c r="A21" s="81"/>
+      <c r="B21" s="82" t="s">
         <v>15</v>
       </c>
       <c r="C21" s="6">
@@ -2235,8 +2242,8 @@
       </c>
     </row>
     <row r="22" spans="1:16">
-      <c r="A22" s="80"/>
-      <c r="B22" s="79"/>
+      <c r="A22" s="81"/>
+      <c r="B22" s="82"/>
       <c r="C22" s="6">
         <v>0.1048</v>
       </c>
@@ -2281,8 +2288,8 @@
       </c>
     </row>
     <row r="23" spans="1:16">
-      <c r="A23" s="80"/>
-      <c r="B23" s="79" t="s">
+      <c r="A23" s="81"/>
+      <c r="B23" s="82" t="s">
         <v>17</v>
       </c>
       <c r="C23" s="6">
@@ -2329,8 +2336,8 @@
       </c>
     </row>
     <row r="24" spans="1:16">
-      <c r="A24" s="80"/>
-      <c r="B24" s="79"/>
+      <c r="A24" s="81"/>
+      <c r="B24" s="82"/>
       <c r="C24">
         <v>0.04</v>
       </c>
@@ -2375,8 +2382,8 @@
       </c>
     </row>
     <row r="25" spans="1:16">
-      <c r="A25" s="80"/>
-      <c r="B25" s="79" t="s">
+      <c r="A25" s="81"/>
+      <c r="B25" s="82" t="s">
         <v>18</v>
       </c>
       <c r="C25" s="6">
@@ -2423,8 +2430,8 @@
       </c>
     </row>
     <row r="26" spans="1:16">
-      <c r="A26" s="80"/>
-      <c r="B26" s="79"/>
+      <c r="A26" s="81"/>
+      <c r="B26" s="82"/>
       <c r="C26">
         <v>5.1999999999999998E-2</v>
       </c>
@@ -2469,8 +2476,8 @@
       </c>
     </row>
     <row r="27" spans="1:16">
-      <c r="A27" s="80"/>
-      <c r="B27" s="79" t="s">
+      <c r="A27" s="81"/>
+      <c r="B27" s="82" t="s">
         <v>19</v>
       </c>
       <c r="C27">
@@ -2517,8 +2524,8 @@
       </c>
     </row>
     <row r="28" spans="1:16">
-      <c r="A28" s="80"/>
-      <c r="B28" s="79"/>
+      <c r="A28" s="81"/>
+      <c r="B28" s="82"/>
       <c r="C28">
         <v>3.5000000000000003E-2</v>
       </c>
@@ -2563,10 +2570,10 @@
       </c>
     </row>
     <row r="30" spans="1:16">
-      <c r="A30" s="80" t="s">
+      <c r="A30" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="79" t="s">
+      <c r="B30" s="82" t="s">
         <v>16</v>
       </c>
       <c r="C30" s="6">
@@ -2613,8 +2620,8 @@
       </c>
     </row>
     <row r="31" spans="1:16">
-      <c r="A31" s="80"/>
-      <c r="B31" s="79"/>
+      <c r="A31" s="81"/>
+      <c r="B31" s="82"/>
       <c r="C31" s="6">
         <v>0.53333333333333399</v>
       </c>
@@ -2659,8 +2666,8 @@
       </c>
     </row>
     <row r="32" spans="1:16">
-      <c r="A32" s="80"/>
-      <c r="B32" s="79" t="s">
+      <c r="A32" s="81"/>
+      <c r="B32" s="82" t="s">
         <v>15</v>
       </c>
       <c r="C32" s="6">
@@ -2707,8 +2714,8 @@
       </c>
     </row>
     <row r="33" spans="1:17">
-      <c r="A33" s="80"/>
-      <c r="B33" s="79"/>
+      <c r="A33" s="81"/>
+      <c r="B33" s="82"/>
       <c r="C33" s="6">
         <v>0.28399999999999997</v>
       </c>
@@ -2753,8 +2760,8 @@
       </c>
     </row>
     <row r="34" spans="1:17">
-      <c r="A34" s="80"/>
-      <c r="B34" s="79" t="s">
+      <c r="A34" s="81"/>
+      <c r="B34" s="82" t="s">
         <v>17</v>
       </c>
       <c r="C34" s="6">
@@ -2801,8 +2808,8 @@
       </c>
     </row>
     <row r="35" spans="1:17">
-      <c r="A35" s="80"/>
-      <c r="B35" s="79"/>
+      <c r="A35" s="81"/>
+      <c r="B35" s="82"/>
       <c r="C35" s="6">
         <v>8.7500000000000105E-2</v>
       </c>
@@ -2847,8 +2854,8 @@
       </c>
     </row>
     <row r="36" spans="1:17">
-      <c r="A36" s="80"/>
-      <c r="B36" s="79" t="s">
+      <c r="A36" s="81"/>
+      <c r="B36" s="82" t="s">
         <v>18</v>
       </c>
       <c r="C36" s="6">
@@ -2895,8 +2902,8 @@
       </c>
     </row>
     <row r="37" spans="1:17">
-      <c r="A37" s="80"/>
-      <c r="B37" s="79"/>
+      <c r="A37" s="81"/>
+      <c r="B37" s="82"/>
       <c r="C37" s="6">
         <v>0.14000000000000001</v>
       </c>
@@ -2941,8 +2948,8 @@
       </c>
     </row>
     <row r="38" spans="1:17">
-      <c r="A38" s="80"/>
-      <c r="B38" s="79" t="s">
+      <c r="A38" s="81"/>
+      <c r="B38" s="82" t="s">
         <v>19</v>
       </c>
       <c r="C38" s="6">
@@ -2989,8 +2996,8 @@
       </c>
     </row>
     <row r="39" spans="1:17">
-      <c r="A39" s="80"/>
-      <c r="B39" s="79"/>
+      <c r="A39" s="81"/>
+      <c r="B39" s="82"/>
       <c r="C39" s="6">
         <v>0.22500000000000001</v>
       </c>
@@ -3147,10 +3154,10 @@
       </c>
     </row>
     <row r="43" spans="1:17">
-      <c r="A43" s="80" t="s">
+      <c r="A43" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="79" t="s">
+      <c r="B43" s="82" t="s">
         <v>16</v>
       </c>
       <c r="C43" s="4">
@@ -3197,8 +3204,8 @@
       </c>
     </row>
     <row r="44" spans="1:17">
-      <c r="A44" s="80"/>
-      <c r="B44" s="79"/>
+      <c r="A44" s="81"/>
+      <c r="B44" s="82"/>
       <c r="C44" s="4">
         <v>0.35929627778837298</v>
       </c>
@@ -3243,8 +3250,8 @@
       </c>
     </row>
     <row r="45" spans="1:17">
-      <c r="A45" s="80"/>
-      <c r="B45" s="79" t="s">
+      <c r="A45" s="81"/>
+      <c r="B45" s="82" t="s">
         <v>15</v>
       </c>
       <c r="C45" s="4">
@@ -3291,8 +3298,8 @@
       </c>
     </row>
     <row r="46" spans="1:17">
-      <c r="A46" s="80"/>
-      <c r="B46" s="79"/>
+      <c r="A46" s="81"/>
+      <c r="B46" s="82"/>
       <c r="C46" s="4">
         <v>0.11918811759426499</v>
       </c>
@@ -3337,8 +3344,8 @@
       </c>
     </row>
     <row r="47" spans="1:17">
-      <c r="A47" s="80"/>
-      <c r="B47" s="79" t="s">
+      <c r="A47" s="81"/>
+      <c r="B47" s="82" t="s">
         <v>17</v>
       </c>
       <c r="C47" s="4">
@@ -3385,8 +3392,8 @@
       </c>
     </row>
     <row r="48" spans="1:17">
-      <c r="A48" s="80"/>
-      <c r="B48" s="79"/>
+      <c r="A48" s="81"/>
+      <c r="B48" s="82"/>
       <c r="C48">
         <v>4.1451873192934301E-2</v>
       </c>
@@ -3431,8 +3438,8 @@
       </c>
     </row>
     <row r="49" spans="1:16">
-      <c r="A49" s="80"/>
-      <c r="B49" s="79" t="s">
+      <c r="A49" s="81"/>
+      <c r="B49" s="82" t="s">
         <v>18</v>
       </c>
       <c r="C49">
@@ -3479,8 +3486,8 @@
       </c>
     </row>
     <row r="50" spans="1:16">
-      <c r="A50" s="80"/>
-      <c r="B50" s="79"/>
+      <c r="A50" s="81"/>
+      <c r="B50" s="82"/>
       <c r="C50">
         <v>2.2165294764432301E-2</v>
       </c>
@@ -3525,8 +3532,8 @@
       </c>
     </row>
     <row r="51" spans="1:16">
-      <c r="A51" s="80"/>
-      <c r="B51" s="79" t="s">
+      <c r="A51" s="81"/>
+      <c r="B51" s="82" t="s">
         <v>19</v>
       </c>
       <c r="C51">
@@ -3573,8 +3580,8 @@
       </c>
     </row>
     <row r="52" spans="1:16">
-      <c r="A52" s="80"/>
-      <c r="B52" s="79"/>
+      <c r="A52" s="81"/>
+      <c r="B52" s="82"/>
       <c r="C52">
         <v>1.9783438855451401E-2</v>
       </c>
@@ -3619,10 +3626,10 @@
       </c>
     </row>
     <row r="54" spans="1:16">
-      <c r="A54" s="80" t="s">
+      <c r="A54" s="81" t="s">
         <v>26</v>
       </c>
-      <c r="B54" s="79" t="s">
+      <c r="B54" s="82" t="s">
         <v>16</v>
       </c>
       <c r="C54" s="4">
@@ -3669,8 +3676,8 @@
       </c>
     </row>
     <row r="55" spans="1:16">
-      <c r="A55" s="80"/>
-      <c r="B55" s="79"/>
+      <c r="A55" s="81"/>
+      <c r="B55" s="82"/>
       <c r="C55" s="4">
         <v>0.36</v>
       </c>
@@ -3715,8 +3722,8 @@
       </c>
     </row>
     <row r="56" spans="1:16">
-      <c r="A56" s="80"/>
-      <c r="B56" s="79" t="s">
+      <c r="A56" s="81"/>
+      <c r="B56" s="82" t="s">
         <v>15</v>
       </c>
       <c r="C56" s="4">
@@ -3763,8 +3770,8 @@
       </c>
     </row>
     <row r="57" spans="1:16">
-      <c r="A57" s="80"/>
-      <c r="B57" s="79"/>
+      <c r="A57" s="81"/>
+      <c r="B57" s="82"/>
       <c r="C57" s="4">
         <v>0.26</v>
       </c>
@@ -3809,8 +3816,8 @@
       </c>
     </row>
     <row r="58" spans="1:16">
-      <c r="A58" s="80"/>
-      <c r="B58" s="79" t="s">
+      <c r="A58" s="81"/>
+      <c r="B58" s="82" t="s">
         <v>17</v>
       </c>
       <c r="C58" s="4">
@@ -3857,8 +3864,8 @@
       </c>
     </row>
     <row r="59" spans="1:16">
-      <c r="A59" s="80"/>
-      <c r="B59" s="79"/>
+      <c r="A59" s="81"/>
+      <c r="B59" s="82"/>
       <c r="C59" s="4">
         <v>8.0000000000000099E-2</v>
       </c>
@@ -3903,8 +3910,8 @@
       </c>
     </row>
     <row r="60" spans="1:16">
-      <c r="A60" s="80"/>
-      <c r="B60" s="79" t="s">
+      <c r="A60" s="81"/>
+      <c r="B60" s="82" t="s">
         <v>18</v>
       </c>
       <c r="C60" s="4">
@@ -3951,8 +3958,8 @@
       </c>
     </row>
     <row r="61" spans="1:16">
-      <c r="A61" s="80"/>
-      <c r="B61" s="79"/>
+      <c r="A61" s="81"/>
+      <c r="B61" s="82"/>
       <c r="C61" s="4">
         <v>0.1</v>
       </c>
@@ -3997,8 +4004,8 @@
       </c>
     </row>
     <row r="62" spans="1:16">
-      <c r="A62" s="80"/>
-      <c r="B62" s="79" t="s">
+      <c r="A62" s="81"/>
+      <c r="B62" s="82" t="s">
         <v>19</v>
       </c>
       <c r="C62" s="4">
@@ -4045,8 +4052,8 @@
       </c>
     </row>
     <row r="63" spans="1:16">
-      <c r="A63" s="80"/>
-      <c r="B63" s="79"/>
+      <c r="A63" s="81"/>
+      <c r="B63" s="82"/>
       <c r="C63" s="4">
         <v>0.1</v>
       </c>
@@ -4092,24 +4099,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A30:A39"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="A7:A17"/>
-    <mergeCell ref="A19:A28"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B19:B20"/>
     <mergeCell ref="B62:B63"/>
     <mergeCell ref="A54:A63"/>
     <mergeCell ref="A43:A52"/>
@@ -4122,6 +4111,24 @@
     <mergeCell ref="B47:B48"/>
     <mergeCell ref="B49:B50"/>
     <mergeCell ref="B51:B52"/>
+    <mergeCell ref="A7:A17"/>
+    <mergeCell ref="A19:A28"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="A30:A39"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B38:B39"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4133,45 +4140,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:LB86"/>
   <sheetViews>
-    <sheetView topLeftCell="B55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+    <sheetView topLeftCell="B19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="2:314">
-      <c r="D1" s="79" t="s">
+      <c r="D1" s="97" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
-      <c r="M1" s="79"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="82"/>
+      <c r="M1" s="82"/>
     </row>
     <row r="2" spans="2:314">
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
-      <c r="M2" s="79"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="82"/>
+      <c r="L2" s="82"/>
+      <c r="M2" s="82"/>
     </row>
     <row r="3" spans="2:314">
-      <c r="D3" s="79" t="s">
-        <v>117</v>
-      </c>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
+      <c r="D3" s="82" t="s">
+        <v>116</v>
+      </c>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
     </row>
     <row r="4" spans="2:314">
       <c r="C4" s="53" t="s">
@@ -4273,7 +4280,7 @@
       </c>
     </row>
     <row r="7" spans="2:314">
-      <c r="B7" s="80" t="s">
+      <c r="B7" s="81" t="s">
         <v>39</v>
       </c>
       <c r="C7" s="51">
@@ -4977,7 +4984,7 @@
       </c>
     </row>
     <row r="8" spans="2:314" ht="14.25" customHeight="1">
-      <c r="B8" s="80"/>
+      <c r="B8" s="81"/>
       <c r="C8" s="52">
         <v>2</v>
       </c>
@@ -5916,7 +5923,7 @@
       </c>
     </row>
     <row r="9" spans="2:314">
-      <c r="B9" s="80"/>
+      <c r="B9" s="81"/>
       <c r="C9" s="51">
         <v>3</v>
       </c>
@@ -6855,7 +6862,7 @@
       </c>
     </row>
     <row r="10" spans="2:314">
-      <c r="B10" s="80"/>
+      <c r="B10" s="81"/>
       <c r="C10" s="52">
         <v>4</v>
       </c>
@@ -7794,7 +7801,7 @@
       </c>
     </row>
     <row r="11" spans="2:314">
-      <c r="B11" s="80"/>
+      <c r="B11" s="81"/>
       <c r="C11" s="51">
         <v>5</v>
       </c>
@@ -8733,7 +8740,7 @@
       </c>
     </row>
     <row r="12" spans="2:314">
-      <c r="B12" s="80"/>
+      <c r="B12" s="81"/>
       <c r="C12" s="52">
         <v>6</v>
       </c>
@@ -9672,7 +9679,7 @@
       </c>
     </row>
     <row r="13" spans="2:314">
-      <c r="B13" s="80"/>
+      <c r="B13" s="81"/>
       <c r="C13" s="51">
         <v>7</v>
       </c>
@@ -10611,7 +10618,7 @@
       </c>
     </row>
     <row r="14" spans="2:314">
-      <c r="B14" s="80"/>
+      <c r="B14" s="81"/>
       <c r="C14" s="52">
         <v>8</v>
       </c>
@@ -11550,7 +11557,7 @@
       </c>
     </row>
     <row r="15" spans="2:314">
-      <c r="B15" s="80"/>
+      <c r="B15" s="81"/>
       <c r="C15" s="51">
         <v>9</v>
       </c>
@@ -12489,7 +12496,7 @@
       </c>
     </row>
     <row r="16" spans="2:314">
-      <c r="B16" s="80"/>
+      <c r="B16" s="81"/>
       <c r="C16" s="52">
         <v>10</v>
       </c>
@@ -13428,7 +13435,7 @@
       </c>
     </row>
     <row r="17" spans="2:314">
-      <c r="B17" s="80"/>
+      <c r="B17" s="81"/>
       <c r="C17" s="51">
         <v>11</v>
       </c>
@@ -14367,7 +14374,7 @@
       </c>
     </row>
     <row r="18" spans="2:314">
-      <c r="B18" s="80"/>
+      <c r="B18" s="81"/>
       <c r="C18" s="52">
         <v>12</v>
       </c>
@@ -15306,7 +15313,7 @@
       </c>
     </row>
     <row r="19" spans="2:314">
-      <c r="B19" s="80"/>
+      <c r="B19" s="81"/>
       <c r="C19" s="51">
         <v>13</v>
       </c>
@@ -16245,7 +16252,7 @@
       </c>
     </row>
     <row r="20" spans="2:314">
-      <c r="B20" s="80"/>
+      <c r="B20" s="81"/>
       <c r="C20" s="52">
         <v>14</v>
       </c>
@@ -17184,12 +17191,12 @@
       </c>
     </row>
     <row r="23" spans="2:314">
-      <c r="D23" s="79" t="s">
+      <c r="D23" s="82" t="s">
         <v>41</v>
       </c>
-      <c r="E23" s="79"/>
-      <c r="F23" s="79"/>
-      <c r="G23" s="79"/>
+      <c r="E23" s="82"/>
+      <c r="F23" s="82"/>
+      <c r="G23" s="82"/>
     </row>
     <row r="24" spans="2:314">
       <c r="C24" s="53" t="s">
@@ -17291,7 +17298,7 @@
       </c>
     </row>
     <row r="27" spans="2:314">
-      <c r="B27" s="80" t="s">
+      <c r="B27" s="81" t="s">
         <v>39</v>
       </c>
       <c r="C27" s="51">
@@ -17836,7 +17843,7 @@
       </c>
     </row>
     <row r="28" spans="2:314">
-      <c r="B28" s="80"/>
+      <c r="B28" s="81"/>
       <c r="C28" s="52">
         <v>2</v>
       </c>
@@ -18379,7 +18386,7 @@
       </c>
     </row>
     <row r="29" spans="2:314">
-      <c r="B29" s="80"/>
+      <c r="B29" s="81"/>
       <c r="C29" s="51">
         <v>3</v>
       </c>
@@ -18922,7 +18929,7 @@
       </c>
     </row>
     <row r="30" spans="2:314">
-      <c r="B30" s="80"/>
+      <c r="B30" s="81"/>
       <c r="C30" s="52">
         <v>4</v>
       </c>
@@ -19465,7 +19472,7 @@
       </c>
     </row>
     <row r="31" spans="2:314">
-      <c r="B31" s="80"/>
+      <c r="B31" s="81"/>
       <c r="C31" s="51">
         <v>5</v>
       </c>
@@ -20008,7 +20015,7 @@
       </c>
     </row>
     <row r="32" spans="2:314">
-      <c r="B32" s="80"/>
+      <c r="B32" s="81"/>
       <c r="C32" s="52">
         <v>6</v>
       </c>
@@ -20551,7 +20558,7 @@
       </c>
     </row>
     <row r="33" spans="2:182">
-      <c r="B33" s="80"/>
+      <c r="B33" s="81"/>
       <c r="C33" s="51">
         <v>7</v>
       </c>
@@ -21094,7 +21101,7 @@
       </c>
     </row>
     <row r="34" spans="2:182">
-      <c r="B34" s="80"/>
+      <c r="B34" s="81"/>
       <c r="C34" s="52">
         <v>8</v>
       </c>
@@ -21637,7 +21644,7 @@
       </c>
     </row>
     <row r="35" spans="2:182">
-      <c r="B35" s="80"/>
+      <c r="B35" s="81"/>
       <c r="C35" s="51">
         <v>9</v>
       </c>
@@ -22180,7 +22187,7 @@
       </c>
     </row>
     <row r="36" spans="2:182">
-      <c r="B36" s="80"/>
+      <c r="B36" s="81"/>
       <c r="C36" s="52">
         <v>10</v>
       </c>
@@ -22723,7 +22730,7 @@
       </c>
     </row>
     <row r="37" spans="2:182">
-      <c r="B37" s="80"/>
+      <c r="B37" s="81"/>
       <c r="C37" s="51">
         <v>11</v>
       </c>
@@ -23266,7 +23273,7 @@
       </c>
     </row>
     <row r="38" spans="2:182">
-      <c r="B38" s="80"/>
+      <c r="B38" s="81"/>
       <c r="C38" s="52">
         <v>12</v>
       </c>
@@ -23809,7 +23816,7 @@
       </c>
     </row>
     <row r="39" spans="2:182">
-      <c r="B39" s="80"/>
+      <c r="B39" s="81"/>
       <c r="C39" s="51">
         <v>13</v>
       </c>
@@ -24352,7 +24359,7 @@
       </c>
     </row>
     <row r="40" spans="2:182">
-      <c r="B40" s="80"/>
+      <c r="B40" s="81"/>
       <c r="C40" s="52">
         <v>14</v>
       </c>
@@ -24895,12 +24902,12 @@
       </c>
     </row>
     <row r="43" spans="2:182">
-      <c r="D43" s="79" t="s">
+      <c r="D43" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="E43" s="79"/>
-      <c r="F43" s="79"/>
-      <c r="G43" s="79"/>
+      <c r="E43" s="82"/>
+      <c r="F43" s="82"/>
+      <c r="G43" s="82"/>
     </row>
     <row r="44" spans="2:182">
       <c r="C44" s="53" t="s">
@@ -25413,7 +25420,7 @@
       </c>
     </row>
     <row r="47" spans="2:182">
-      <c r="B47" s="80" t="s">
+      <c r="B47" s="81" t="s">
         <v>39</v>
       </c>
       <c r="C47" s="51">
@@ -25832,7 +25839,7 @@
       </c>
     </row>
     <row r="48" spans="2:182">
-      <c r="B48" s="80"/>
+      <c r="B48" s="81"/>
       <c r="C48" s="52">
         <v>2</v>
       </c>
@@ -26249,7 +26256,7 @@
       </c>
     </row>
     <row r="49" spans="2:140">
-      <c r="B49" s="80"/>
+      <c r="B49" s="81"/>
       <c r="C49" s="51">
         <v>3</v>
       </c>
@@ -26666,7 +26673,7 @@
       </c>
     </row>
     <row r="50" spans="2:140">
-      <c r="B50" s="80"/>
+      <c r="B50" s="81"/>
       <c r="C50" s="52">
         <v>4</v>
       </c>
@@ -27083,7 +27090,7 @@
       </c>
     </row>
     <row r="51" spans="2:140">
-      <c r="B51" s="80"/>
+      <c r="B51" s="81"/>
       <c r="C51" s="51">
         <v>5</v>
       </c>
@@ -27500,7 +27507,7 @@
       </c>
     </row>
     <row r="52" spans="2:140">
-      <c r="B52" s="80"/>
+      <c r="B52" s="81"/>
       <c r="C52" s="52">
         <v>6</v>
       </c>
@@ -27917,7 +27924,7 @@
       </c>
     </row>
     <row r="53" spans="2:140">
-      <c r="B53" s="80"/>
+      <c r="B53" s="81"/>
       <c r="C53" s="51">
         <v>7</v>
       </c>
@@ -28334,7 +28341,7 @@
       </c>
     </row>
     <row r="54" spans="2:140">
-      <c r="B54" s="80"/>
+      <c r="B54" s="81"/>
       <c r="C54" s="52">
         <v>8</v>
       </c>
@@ -28751,7 +28758,7 @@
       </c>
     </row>
     <row r="55" spans="2:140">
-      <c r="B55" s="80"/>
+      <c r="B55" s="81"/>
       <c r="C55" s="51">
         <v>9</v>
       </c>
@@ -29168,7 +29175,7 @@
       </c>
     </row>
     <row r="56" spans="2:140">
-      <c r="B56" s="80"/>
+      <c r="B56" s="81"/>
       <c r="C56" s="52">
         <v>10</v>
       </c>
@@ -29585,7 +29592,7 @@
       </c>
     </row>
     <row r="57" spans="2:140">
-      <c r="B57" s="80"/>
+      <c r="B57" s="81"/>
       <c r="C57" s="51">
         <v>11</v>
       </c>
@@ -30002,7 +30009,7 @@
       </c>
     </row>
     <row r="58" spans="2:140">
-      <c r="B58" s="80"/>
+      <c r="B58" s="81"/>
       <c r="C58" s="52">
         <v>12</v>
       </c>
@@ -30419,7 +30426,7 @@
       </c>
     </row>
     <row r="59" spans="2:140">
-      <c r="B59" s="80"/>
+      <c r="B59" s="81"/>
       <c r="C59" s="51">
         <v>13</v>
       </c>
@@ -30836,27 +30843,27 @@
       </c>
     </row>
     <row r="60" spans="2:140">
-      <c r="B60" s="80"/>
+      <c r="B60" s="81"/>
       <c r="C60" s="52">
         <v>14</v>
       </c>
     </row>
     <row r="67" spans="2:88">
-      <c r="B67" s="81" t="s">
+      <c r="B67" s="83" t="s">
         <v>44</v>
       </c>
-      <c r="C67" s="79"/>
-      <c r="D67" s="79"/>
-      <c r="E67" s="79"/>
-      <c r="F67" s="79"/>
+      <c r="C67" s="82"/>
+      <c r="D67" s="82"/>
+      <c r="E67" s="82"/>
+      <c r="F67" s="82"/>
     </row>
     <row r="69" spans="2:88">
-      <c r="D69" s="79" t="s">
+      <c r="D69" s="82" t="s">
         <v>56</v>
       </c>
-      <c r="E69" s="79"/>
-      <c r="F69" s="79"/>
-      <c r="G69" s="79"/>
+      <c r="E69" s="82"/>
+      <c r="F69" s="82"/>
+      <c r="G69" s="82"/>
     </row>
     <row r="70" spans="2:88">
       <c r="C70" s="53" t="s">
@@ -30978,7 +30985,7 @@
       <c r="CJ72" s="10"/>
     </row>
     <row r="73" spans="2:88">
-      <c r="B73" s="80" t="s">
+      <c r="B73" s="81" t="s">
         <v>39</v>
       </c>
       <c r="C73" s="51">
@@ -31213,7 +31220,7 @@
       <c r="CJ73" s="10"/>
     </row>
     <row r="74" spans="2:88">
-      <c r="B74" s="80"/>
+      <c r="B74" s="81"/>
       <c r="C74" s="52">
         <v>2</v>
       </c>
@@ -31446,7 +31453,7 @@
       <c r="CJ74" s="10"/>
     </row>
     <row r="75" spans="2:88">
-      <c r="B75" s="80"/>
+      <c r="B75" s="81"/>
       <c r="C75" s="51">
         <v>3</v>
       </c>
@@ -31679,7 +31686,7 @@
       <c r="CJ75" s="10"/>
     </row>
     <row r="76" spans="2:88">
-      <c r="B76" s="80"/>
+      <c r="B76" s="81"/>
       <c r="C76" s="52">
         <v>4</v>
       </c>
@@ -31912,7 +31919,7 @@
       <c r="CJ76" s="10"/>
     </row>
     <row r="77" spans="2:88">
-      <c r="B77" s="80"/>
+      <c r="B77" s="81"/>
       <c r="C77" s="51">
         <v>5</v>
       </c>
@@ -32145,7 +32152,7 @@
       <c r="CJ77" s="10"/>
     </row>
     <row r="78" spans="2:88">
-      <c r="B78" s="80"/>
+      <c r="B78" s="81"/>
       <c r="C78" s="52">
         <v>6</v>
       </c>
@@ -32378,7 +32385,7 @@
       <c r="CJ78" s="10"/>
     </row>
     <row r="79" spans="2:88">
-      <c r="B79" s="80"/>
+      <c r="B79" s="81"/>
       <c r="C79" s="51">
         <v>7</v>
       </c>
@@ -32611,7 +32618,7 @@
       <c r="CJ79" s="10"/>
     </row>
     <row r="80" spans="2:88">
-      <c r="B80" s="80"/>
+      <c r="B80" s="81"/>
       <c r="C80" s="52">
         <v>8</v>
       </c>
@@ -32844,7 +32851,7 @@
       <c r="CJ80" s="10"/>
     </row>
     <row r="81" spans="2:88">
-      <c r="B81" s="80"/>
+      <c r="B81" s="81"/>
       <c r="C81" s="51">
         <v>9</v>
       </c>
@@ -33077,7 +33084,7 @@
       <c r="CJ81" s="10"/>
     </row>
     <row r="82" spans="2:88">
-      <c r="B82" s="80"/>
+      <c r="B82" s="81"/>
       <c r="C82" s="52">
         <v>10</v>
       </c>
@@ -33310,7 +33317,7 @@
       <c r="CJ82" s="10"/>
     </row>
     <row r="83" spans="2:88">
-      <c r="B83" s="80"/>
+      <c r="B83" s="81"/>
       <c r="C83" s="51">
         <v>11</v>
       </c>
@@ -33543,7 +33550,7 @@
       <c r="CJ83" s="10"/>
     </row>
     <row r="84" spans="2:88">
-      <c r="B84" s="80"/>
+      <c r="B84" s="81"/>
       <c r="C84" s="52">
         <v>12</v>
       </c>
@@ -33776,7 +33783,7 @@
       <c r="CJ84" s="10"/>
     </row>
     <row r="85" spans="2:88">
-      <c r="B85" s="80"/>
+      <c r="B85" s="81"/>
       <c r="C85" s="51">
         <v>13</v>
       </c>
@@ -34009,7 +34016,7 @@
       <c r="CJ85" s="10"/>
     </row>
     <row r="86" spans="2:88">
-      <c r="B86" s="80"/>
+      <c r="B86" s="81"/>
       <c r="C86" s="52">
         <v>14</v>
       </c>
@@ -34243,16 +34250,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="D69:G69"/>
+    <mergeCell ref="B73:B86"/>
+    <mergeCell ref="B67:F67"/>
+    <mergeCell ref="D43:G43"/>
+    <mergeCell ref="B47:B60"/>
     <mergeCell ref="D1:M2"/>
     <mergeCell ref="D3:G3"/>
     <mergeCell ref="B7:B20"/>
     <mergeCell ref="D23:G23"/>
     <mergeCell ref="B27:B40"/>
-    <mergeCell ref="D69:G69"/>
-    <mergeCell ref="B73:B86"/>
-    <mergeCell ref="B67:F67"/>
-    <mergeCell ref="D43:G43"/>
-    <mergeCell ref="B47:B60"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -34271,16 +34278,16 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="2" spans="2:15">
-      <c r="B2" s="79" t="s">
+      <c r="B2" s="82" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79" t="s">
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
     </row>
     <row r="3" spans="2:15">
       <c r="B3">
@@ -34371,16 +34378,16 @@
       </c>
     </row>
     <row r="6" spans="2:15">
-      <c r="B6" s="79" t="s">
+      <c r="B6" s="82" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="79"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="79" t="s">
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82" t="s">
         <v>59</v>
       </c>
-      <c r="F6" s="79"/>
-      <c r="G6" s="79"/>
+      <c r="F6" s="82"/>
+      <c r="G6" s="82"/>
     </row>
     <row r="7" spans="2:15">
       <c r="B7">
@@ -34486,8 +34493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:CS94"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F83" sqref="F83"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AB10" sqref="AB10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -44773,8 +44780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD141"/>
   <sheetViews>
-    <sheetView topLeftCell="C82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G114" sqref="G114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -44823,46 +44830,46 @@
       <c r="B3" s="11"/>
       <c r="C3" s="76"/>
       <c r="D3" s="76" t="s">
+        <v>117</v>
+      </c>
+      <c r="E3" s="76" t="s">
         <v>118</v>
       </c>
-      <c r="E3" s="76" t="s">
+      <c r="F3" s="76" t="s">
         <v>119</v>
       </c>
-      <c r="F3" s="76" t="s">
+      <c r="G3" s="76" t="s">
         <v>120</v>
       </c>
-      <c r="G3" s="76" t="s">
+      <c r="H3" s="77" t="s">
         <v>121</v>
       </c>
-      <c r="H3" s="77" t="s">
+      <c r="I3" s="78" t="s">
+        <v>118</v>
+      </c>
+      <c r="J3" s="76" t="s">
         <v>122</v>
       </c>
-      <c r="I3" s="78" t="s">
+      <c r="K3" s="76" t="s">
+        <v>122</v>
+      </c>
+      <c r="L3" s="76" t="s">
+        <v>123</v>
+      </c>
+      <c r="M3" s="76" t="s">
+        <v>124</v>
+      </c>
+      <c r="N3" s="76" t="s">
+        <v>121</v>
+      </c>
+      <c r="O3" s="77" t="s">
+        <v>118</v>
+      </c>
+      <c r="P3" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q3" s="15" t="s">
         <v>119</v>
-      </c>
-      <c r="J3" s="76" t="s">
-        <v>123</v>
-      </c>
-      <c r="K3" s="76" t="s">
-        <v>123</v>
-      </c>
-      <c r="L3" s="76" t="s">
-        <v>124</v>
-      </c>
-      <c r="M3" s="76" t="s">
-        <v>125</v>
-      </c>
-      <c r="N3" s="76" t="s">
-        <v>122</v>
-      </c>
-      <c r="O3" s="77" t="s">
-        <v>119</v>
-      </c>
-      <c r="P3" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q3" s="15" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:17 16384:16384" ht="15" thickBot="1">
@@ -44892,7 +44899,7 @@
       <c r="A5" s="8"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -44912,7 +44919,7 @@
     <row r="6" spans="1:17 16384:16384">
       <c r="A6" s="8"/>
       <c r="B6" s="10"/>
-      <c r="C6" s="82" t="s">
+      <c r="C6" s="92" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="4">
@@ -44961,7 +44968,7 @@
     <row r="7" spans="1:17 16384:16384">
       <c r="A7" s="8"/>
       <c r="B7" s="10"/>
-      <c r="C7" s="83"/>
+      <c r="C7" s="84"/>
       <c r="D7" s="10">
         <v>-0.04</v>
       </c>
@@ -45008,7 +45015,7 @@
     <row r="8" spans="1:17 16384:16384">
       <c r="A8" s="8"/>
       <c r="B8" s="10"/>
-      <c r="C8" s="83" t="s">
+      <c r="C8" s="84" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="4">
@@ -45057,7 +45064,7 @@
     <row r="9" spans="1:17 16384:16384">
       <c r="A9" s="8"/>
       <c r="B9" s="10"/>
-      <c r="C9" s="83"/>
+      <c r="C9" s="84"/>
       <c r="D9" s="4">
         <v>-0.26</v>
       </c>
@@ -45104,7 +45111,7 @@
     <row r="10" spans="1:17 16384:16384">
       <c r="A10" s="8"/>
       <c r="B10" s="10"/>
-      <c r="C10" s="83" t="s">
+      <c r="C10" s="84" t="s">
         <v>17</v>
       </c>
       <c r="D10" s="4">
@@ -45153,7 +45160,7 @@
     <row r="11" spans="1:17 16384:16384">
       <c r="A11" s="8"/>
       <c r="B11" s="10"/>
-      <c r="C11" s="83"/>
+      <c r="C11" s="84"/>
       <c r="D11" s="10">
         <v>-8.0000000000000099E-2</v>
       </c>
@@ -45200,7 +45207,7 @@
     <row r="12" spans="1:17 16384:16384">
       <c r="A12" s="8"/>
       <c r="B12" s="10"/>
-      <c r="C12" s="83" t="s">
+      <c r="C12" s="84" t="s">
         <v>18</v>
       </c>
       <c r="D12" s="4">
@@ -45249,7 +45256,7 @@
     <row r="13" spans="1:17 16384:16384">
       <c r="A13" s="8"/>
       <c r="B13" s="10"/>
-      <c r="C13" s="83"/>
+      <c r="C13" s="84"/>
       <c r="D13" s="4">
         <v>-0.1</v>
       </c>
@@ -45296,7 +45303,7 @@
     <row r="14" spans="1:17 16384:16384">
       <c r="A14" s="8"/>
       <c r="B14" s="10"/>
-      <c r="C14" s="83" t="s">
+      <c r="C14" s="84" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="4">
@@ -45345,7 +45352,7 @@
     <row r="15" spans="1:17 16384:16384">
       <c r="A15" s="8"/>
       <c r="B15" s="10"/>
-      <c r="C15" s="84"/>
+      <c r="C15" s="85"/>
       <c r="D15" s="10">
         <v>-6.0000000000000102E-2</v>
       </c>
@@ -45543,13 +45550,13 @@
       </c>
     </row>
     <row r="21" spans="1:18" ht="15.75" customHeight="1">
-      <c r="A21" s="85" t="s">
+      <c r="A21" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="90" t="s">
+      <c r="B21" s="86" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="82" t="s">
+      <c r="C21" s="92" t="s">
         <v>16</v>
       </c>
       <c r="D21" s="34">
@@ -45599,9 +45606,9 @@
       </c>
     </row>
     <row r="22" spans="1:18">
-      <c r="A22" s="86"/>
-      <c r="B22" s="91"/>
-      <c r="C22" s="83"/>
+      <c r="A22" s="90"/>
+      <c r="B22" s="87"/>
+      <c r="C22" s="84"/>
       <c r="D22" s="35">
         <v>0.36</v>
       </c>
@@ -45649,9 +45656,9 @@
       </c>
     </row>
     <row r="23" spans="1:18">
-      <c r="A23" s="86"/>
-      <c r="B23" s="91"/>
-      <c r="C23" s="83" t="s">
+      <c r="A23" s="90"/>
+      <c r="B23" s="87"/>
+      <c r="C23" s="84" t="s">
         <v>15</v>
       </c>
       <c r="D23" s="35">
@@ -45701,9 +45708,9 @@
       </c>
     </row>
     <row r="24" spans="1:18">
-      <c r="A24" s="86"/>
-      <c r="B24" s="91"/>
-      <c r="C24" s="83"/>
+      <c r="A24" s="90"/>
+      <c r="B24" s="87"/>
+      <c r="C24" s="84"/>
       <c r="D24" s="35">
         <v>0.26</v>
       </c>
@@ -45751,9 +45758,9 @@
       </c>
     </row>
     <row r="25" spans="1:18">
-      <c r="A25" s="86"/>
-      <c r="B25" s="91"/>
-      <c r="C25" s="83" t="s">
+      <c r="A25" s="90"/>
+      <c r="B25" s="87"/>
+      <c r="C25" s="84" t="s">
         <v>17</v>
       </c>
       <c r="D25" s="35">
@@ -45803,9 +45810,9 @@
       </c>
     </row>
     <row r="26" spans="1:18">
-      <c r="A26" s="86"/>
-      <c r="B26" s="91"/>
-      <c r="C26" s="83"/>
+      <c r="A26" s="90"/>
+      <c r="B26" s="87"/>
+      <c r="C26" s="84"/>
       <c r="D26" s="16">
         <v>8.0000000000000099E-2</v>
       </c>
@@ -45853,9 +45860,9 @@
       </c>
     </row>
     <row r="27" spans="1:18">
-      <c r="A27" s="86"/>
-      <c r="B27" s="91"/>
-      <c r="C27" s="83" t="s">
+      <c r="A27" s="90"/>
+      <c r="B27" s="87"/>
+      <c r="C27" s="84" t="s">
         <v>18</v>
       </c>
       <c r="D27" s="35">
@@ -45905,9 +45912,9 @@
       </c>
     </row>
     <row r="28" spans="1:18">
-      <c r="A28" s="86"/>
-      <c r="B28" s="91"/>
-      <c r="C28" s="83"/>
+      <c r="A28" s="90"/>
+      <c r="B28" s="87"/>
+      <c r="C28" s="84"/>
       <c r="D28" s="35">
         <v>0.1</v>
       </c>
@@ -45955,9 +45962,9 @@
       </c>
     </row>
     <row r="29" spans="1:18">
-      <c r="A29" s="86"/>
-      <c r="B29" s="91"/>
-      <c r="C29" s="83" t="s">
+      <c r="A29" s="90"/>
+      <c r="B29" s="87"/>
+      <c r="C29" s="84" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="35">
@@ -46007,9 +46014,9 @@
       </c>
     </row>
     <row r="30" spans="1:18">
-      <c r="A30" s="86"/>
-      <c r="B30" s="92"/>
-      <c r="C30" s="84"/>
+      <c r="A30" s="90"/>
+      <c r="B30" s="88"/>
+      <c r="C30" s="85"/>
       <c r="D30" s="36">
         <v>0.1</v>
       </c>
@@ -46057,11 +46064,11 @@
       </c>
     </row>
     <row r="31" spans="1:18">
-      <c r="A31" s="86"/>
-      <c r="B31" s="88" t="s">
+      <c r="A31" s="90"/>
+      <c r="B31" s="93" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="89"/>
+      <c r="C31" s="94"/>
       <c r="D31" s="43">
         <v>0.875</v>
       </c>
@@ -46107,11 +46114,11 @@
       <c r="R31" s="50"/>
     </row>
     <row r="32" spans="1:18">
-      <c r="A32" s="86"/>
-      <c r="B32" s="90" t="s">
+      <c r="A32" s="90"/>
+      <c r="B32" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="82" t="s">
+      <c r="C32" s="92" t="s">
         <v>16</v>
       </c>
       <c r="D32" s="32">
@@ -46161,9 +46168,9 @@
       </c>
     </row>
     <row r="33" spans="1:18">
-      <c r="A33" s="86"/>
-      <c r="B33" s="91"/>
-      <c r="C33" s="83"/>
+      <c r="A33" s="90"/>
+      <c r="B33" s="87"/>
+      <c r="C33" s="84"/>
       <c r="D33" s="33">
         <v>0.26</v>
       </c>
@@ -46211,9 +46218,9 @@
       </c>
     </row>
     <row r="34" spans="1:18">
-      <c r="A34" s="86"/>
-      <c r="B34" s="91"/>
-      <c r="C34" s="83" t="s">
+      <c r="A34" s="90"/>
+      <c r="B34" s="87"/>
+      <c r="C34" s="84" t="s">
         <v>15</v>
       </c>
       <c r="D34" s="33">
@@ -46263,9 +46270,9 @@
       </c>
     </row>
     <row r="35" spans="1:18">
-      <c r="A35" s="86"/>
-      <c r="B35" s="91"/>
-      <c r="C35" s="83"/>
+      <c r="A35" s="90"/>
+      <c r="B35" s="87"/>
+      <c r="C35" s="84"/>
       <c r="D35" s="33">
         <v>0.26</v>
       </c>
@@ -46313,9 +46320,9 @@
       </c>
     </row>
     <row r="36" spans="1:18">
-      <c r="A36" s="86"/>
-      <c r="B36" s="91"/>
-      <c r="C36" s="83" t="s">
+      <c r="A36" s="90"/>
+      <c r="B36" s="87"/>
+      <c r="C36" s="84" t="s">
         <v>17</v>
       </c>
       <c r="D36" s="33">
@@ -46365,9 +46372,9 @@
       </c>
     </row>
     <row r="37" spans="1:18">
-      <c r="A37" s="86"/>
-      <c r="B37" s="91"/>
-      <c r="C37" s="83"/>
+      <c r="A37" s="90"/>
+      <c r="B37" s="87"/>
+      <c r="C37" s="84"/>
       <c r="D37" s="31">
         <v>8.0000000000000099E-2</v>
       </c>
@@ -46415,9 +46422,9 @@
       </c>
     </row>
     <row r="38" spans="1:18">
-      <c r="A38" s="86"/>
-      <c r="B38" s="91"/>
-      <c r="C38" s="83" t="s">
+      <c r="A38" s="90"/>
+      <c r="B38" s="87"/>
+      <c r="C38" s="84" t="s">
         <v>18</v>
       </c>
       <c r="D38" s="33">
@@ -46467,9 +46474,9 @@
       </c>
     </row>
     <row r="39" spans="1:18">
-      <c r="A39" s="86"/>
-      <c r="B39" s="91"/>
-      <c r="C39" s="83"/>
+      <c r="A39" s="90"/>
+      <c r="B39" s="87"/>
+      <c r="C39" s="84"/>
       <c r="D39" s="33">
         <v>0.1</v>
       </c>
@@ -46517,9 +46524,9 @@
       </c>
     </row>
     <row r="40" spans="1:18">
-      <c r="A40" s="86"/>
-      <c r="B40" s="91"/>
-      <c r="C40" s="83" t="s">
+      <c r="A40" s="90"/>
+      <c r="B40" s="87"/>
+      <c r="C40" s="84" t="s">
         <v>19</v>
       </c>
       <c r="D40" s="33">
@@ -46569,9 +46576,9 @@
       </c>
     </row>
     <row r="41" spans="1:18">
-      <c r="A41" s="86"/>
-      <c r="B41" s="92"/>
-      <c r="C41" s="84"/>
+      <c r="A41" s="90"/>
+      <c r="B41" s="88"/>
+      <c r="C41" s="85"/>
       <c r="D41" s="26">
         <v>0.04</v>
       </c>
@@ -46619,16 +46626,16 @@
       </c>
     </row>
     <row r="42" spans="1:18">
-      <c r="A42" s="86"/>
+      <c r="A42" s="90"/>
       <c r="B42" s="42"/>
       <c r="R42" s="49"/>
     </row>
     <row r="43" spans="1:18">
-      <c r="A43" s="86"/>
-      <c r="B43" s="90" t="s">
+      <c r="A43" s="90"/>
+      <c r="B43" s="86" t="s">
         <v>33</v>
       </c>
-      <c r="C43" s="82" t="s">
+      <c r="C43" s="92" t="s">
         <v>16</v>
       </c>
       <c r="D43" s="32">
@@ -46678,9 +46685,9 @@
       </c>
     </row>
     <row r="44" spans="1:18">
-      <c r="A44" s="86"/>
-      <c r="B44" s="91"/>
-      <c r="C44" s="83"/>
+      <c r="A44" s="90"/>
+      <c r="B44" s="87"/>
+      <c r="C44" s="84"/>
       <c r="D44" s="33">
         <v>0.36</v>
       </c>
@@ -46728,9 +46735,9 @@
       </c>
     </row>
     <row r="45" spans="1:18">
-      <c r="A45" s="86"/>
-      <c r="B45" s="91"/>
-      <c r="C45" s="83" t="s">
+      <c r="A45" s="90"/>
+      <c r="B45" s="87"/>
+      <c r="C45" s="84" t="s">
         <v>15</v>
       </c>
       <c r="D45" s="33">
@@ -46780,9 +46787,9 @@
       </c>
     </row>
     <row r="46" spans="1:18">
-      <c r="A46" s="86"/>
-      <c r="B46" s="91"/>
-      <c r="C46" s="83"/>
+      <c r="A46" s="90"/>
+      <c r="B46" s="87"/>
+      <c r="C46" s="84"/>
       <c r="D46" s="33">
         <v>0.26</v>
       </c>
@@ -46830,9 +46837,9 @@
       </c>
     </row>
     <row r="47" spans="1:18">
-      <c r="A47" s="86"/>
-      <c r="B47" s="91"/>
-      <c r="C47" s="83" t="s">
+      <c r="A47" s="90"/>
+      <c r="B47" s="87"/>
+      <c r="C47" s="84" t="s">
         <v>17</v>
       </c>
       <c r="D47" s="33">
@@ -46882,9 +46889,9 @@
       </c>
     </row>
     <row r="48" spans="1:18">
-      <c r="A48" s="86"/>
-      <c r="B48" s="91"/>
-      <c r="C48" s="83"/>
+      <c r="A48" s="90"/>
+      <c r="B48" s="87"/>
+      <c r="C48" s="84"/>
       <c r="D48" s="31">
         <v>8.0000000000000099E-2</v>
       </c>
@@ -46932,9 +46939,9 @@
       </c>
     </row>
     <row r="49" spans="1:18">
-      <c r="A49" s="86"/>
-      <c r="B49" s="91"/>
-      <c r="C49" s="83" t="s">
+      <c r="A49" s="90"/>
+      <c r="B49" s="87"/>
+      <c r="C49" s="84" t="s">
         <v>18</v>
       </c>
       <c r="D49" s="33">
@@ -46984,9 +46991,9 @@
       </c>
     </row>
     <row r="50" spans="1:18">
-      <c r="A50" s="86"/>
-      <c r="B50" s="91"/>
-      <c r="C50" s="83"/>
+      <c r="A50" s="90"/>
+      <c r="B50" s="87"/>
+      <c r="C50" s="84"/>
       <c r="D50" s="33">
         <v>0.1</v>
       </c>
@@ -47034,9 +47041,9 @@
       </c>
     </row>
     <row r="51" spans="1:18">
-      <c r="A51" s="86"/>
-      <c r="B51" s="91"/>
-      <c r="C51" s="83" t="s">
+      <c r="A51" s="90"/>
+      <c r="B51" s="87"/>
+      <c r="C51" s="84" t="s">
         <v>19</v>
       </c>
       <c r="D51" s="33">
@@ -47086,9 +47093,9 @@
       </c>
     </row>
     <row r="52" spans="1:18">
-      <c r="A52" s="87"/>
-      <c r="B52" s="92"/>
-      <c r="C52" s="84"/>
+      <c r="A52" s="91"/>
+      <c r="B52" s="88"/>
+      <c r="C52" s="85"/>
       <c r="D52" s="26">
         <v>0.04</v>
       </c>
@@ -47242,7 +47249,7 @@
     </row>
     <row r="64" spans="1:18">
       <c r="O64" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="66" spans="3:17">
@@ -47690,7 +47697,7 @@
     </row>
     <row r="78" spans="3:17">
       <c r="C78" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
     </row>
     <row r="79" spans="3:17">
@@ -48714,7 +48721,7 @@
     </row>
     <row r="108" spans="3:17">
       <c r="C108" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D108" s="4">
         <v>1.4</v>
@@ -49157,7 +49164,7 @@
     </row>
     <row r="120" spans="3:17">
       <c r="C120" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D120" s="4">
         <v>-0.80000000000000104</v>
@@ -49996,6 +50003,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C14:C15"/>
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="C29:C30"/>
     <mergeCell ref="B21:B30"/>
@@ -50012,15 +50028,6 @@
     <mergeCell ref="C34:C35"/>
     <mergeCell ref="C36:C37"/>
     <mergeCell ref="C38:C39"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C14:C15"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -50074,10 +50081,10 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="15.75">
-      <c r="B3" s="93">
+      <c r="B3" s="95">
         <v>1</v>
       </c>
-      <c r="C3" s="93">
+      <c r="C3" s="95">
         <v>400</v>
       </c>
       <c r="D3" s="65">
@@ -50109,8 +50116,8 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="15.75">
-      <c r="B4" s="94"/>
-      <c r="C4" s="94"/>
+      <c r="B4" s="96"/>
+      <c r="C4" s="96"/>
       <c r="D4" s="65">
         <v>0.39097222222222222</v>
       </c>
@@ -50128,10 +50135,10 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75">
-      <c r="B5" s="93">
+      <c r="B5" s="95">
         <v>2</v>
       </c>
-      <c r="C5" s="93">
+      <c r="C5" s="95">
         <v>400</v>
       </c>
       <c r="D5" s="65">
@@ -50163,8 +50170,8 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75">
-      <c r="B6" s="94"/>
-      <c r="C6" s="94"/>
+      <c r="B6" s="96"/>
+      <c r="C6" s="96"/>
       <c r="D6" s="65">
         <v>0.40416666666666662</v>
       </c>
@@ -50182,10 +50189,10 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75">
-      <c r="B7" s="93">
+      <c r="B7" s="95">
         <v>3</v>
       </c>
-      <c r="C7" s="93">
+      <c r="C7" s="95">
         <v>800</v>
       </c>
       <c r="D7" s="65">
@@ -50217,8 +50224,8 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75">
-      <c r="B8" s="94"/>
-      <c r="C8" s="94"/>
+      <c r="B8" s="96"/>
+      <c r="C8" s="96"/>
       <c r="D8" s="65">
         <v>0.43055555555555558</v>
       </c>
@@ -50239,10 +50246,10 @@
       <c r="A9" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="93">
+      <c r="B9" s="95">
         <v>4</v>
       </c>
-      <c r="C9" s="93">
+      <c r="C9" s="95">
         <v>300</v>
       </c>
       <c r="D9" s="65">
@@ -50274,8 +50281,8 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75">
-      <c r="B10" s="94"/>
-      <c r="C10" s="94"/>
+      <c r="B10" s="96"/>
+      <c r="C10" s="96"/>
       <c r="D10" s="65">
         <v>0.44722222222222219</v>
       </c>
@@ -50293,10 +50300,10 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75">
-      <c r="B11" s="93">
+      <c r="B11" s="95">
         <v>5</v>
       </c>
-      <c r="C11" s="93">
+      <c r="C11" s="95">
         <v>300</v>
       </c>
       <c r="D11" s="65">
@@ -50328,8 +50335,8 @@
       </c>
     </row>
     <row r="12" spans="1:15" ht="15.75">
-      <c r="B12" s="94"/>
-      <c r="C12" s="94"/>
+      <c r="B12" s="96"/>
+      <c r="C12" s="96"/>
       <c r="D12" s="65">
         <v>0.46180555555555558</v>
       </c>
@@ -50347,13 +50354,13 @@
       </c>
     </row>
     <row r="15" spans="1:15">
-      <c r="B15" s="79" t="s">
+      <c r="B15" s="82" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="79"/>
-      <c r="D15" s="79"/>
-      <c r="E15" s="79"/>
-      <c r="F15" s="79"/>
+      <c r="C15" s="82"/>
+      <c r="D15" s="82"/>
+      <c r="E15" s="82"/>
+      <c r="F15" s="82"/>
     </row>
     <row r="16" spans="1:15">
       <c r="B16" s="56">
@@ -57408,13 +57415,13 @@
       <c r="CE34" s="8"/>
     </row>
     <row r="39" spans="2:208">
-      <c r="B39" s="79" t="s">
+      <c r="B39" s="82" t="s">
         <v>84</v>
       </c>
-      <c r="C39" s="79"/>
-      <c r="D39" s="79"/>
-      <c r="E39" s="79"/>
-      <c r="F39" s="79"/>
+      <c r="C39" s="82"/>
+      <c r="D39" s="82"/>
+      <c r="E39" s="82"/>
+      <c r="F39" s="82"/>
     </row>
     <row r="40" spans="2:208">
       <c r="B40" s="56">
@@ -66227,13 +66234,13 @@
       </c>
     </row>
     <row r="61" spans="2:208">
-      <c r="B61" s="79" t="s">
+      <c r="B61" s="82" t="s">
         <v>105</v>
       </c>
-      <c r="C61" s="79"/>
-      <c r="D61" s="79"/>
-      <c r="E61" s="79"/>
-      <c r="F61" s="79"/>
+      <c r="C61" s="82"/>
+      <c r="D61" s="82"/>
+      <c r="E61" s="82"/>
+      <c r="F61" s="82"/>
     </row>
     <row r="62" spans="2:208">
       <c r="B62" s="56">
@@ -78448,13 +78455,13 @@
       </c>
     </row>
     <row r="83" spans="2:349">
-      <c r="B83" s="79" t="s">
+      <c r="B83" s="82" t="s">
         <v>106</v>
       </c>
-      <c r="C83" s="79"/>
-      <c r="D83" s="79"/>
-      <c r="E83" s="79"/>
-      <c r="F83" s="79"/>
+      <c r="C83" s="82"/>
+      <c r="D83" s="82"/>
+      <c r="E83" s="82"/>
+      <c r="F83" s="82"/>
     </row>
     <row r="84" spans="2:349">
       <c r="B84" s="56">
@@ -93189,13 +93196,13 @@
       </c>
     </row>
     <row r="104" spans="2:349">
-      <c r="B104" s="79" t="s">
+      <c r="B104" s="82" t="s">
         <v>98</v>
       </c>
-      <c r="C104" s="79"/>
-      <c r="D104" s="79"/>
-      <c r="E104" s="79"/>
-      <c r="F104" s="79"/>
+      <c r="C104" s="82"/>
+      <c r="D104" s="82"/>
+      <c r="E104" s="82"/>
+      <c r="F104" s="82"/>
     </row>
     <row r="105" spans="2:349">
       <c r="B105" s="56">
@@ -96843,11 +96850,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="B61:F61"/>
-    <mergeCell ref="B83:F83"/>
-    <mergeCell ref="B104:F104"/>
-    <mergeCell ref="B15:F15"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="B11:B12"/>
@@ -96858,6 +96860,11 @@
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="C11:C12"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B61:F61"/>
+    <mergeCell ref="B83:F83"/>
+    <mergeCell ref="B104:F104"/>
+    <mergeCell ref="B15:F15"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -96869,8 +96876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D1:CI96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="J34" workbookViewId="0">
+      <selection activeCell="J70" sqref="A70:XFD70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -96920,33 +96927,96 @@
       </c>
     </row>
     <row r="2" spans="4:60">
-      <c r="E2" s="95">
+      <c r="E2" s="79">
         <v>1</v>
       </c>
-      <c r="F2" s="96">
+      <c r="F2" s="80">
+        <v>1</v>
+      </c>
+      <c r="G2" s="80">
+        <v>0.8</v>
+      </c>
+      <c r="H2" s="80">
+        <v>1</v>
+      </c>
+      <c r="I2" s="80">
+        <v>1</v>
+      </c>
+      <c r="J2" s="80">
+        <v>1</v>
+      </c>
+      <c r="K2" s="80">
+        <v>1</v>
+      </c>
+      <c r="L2" s="80">
+        <v>0.6</v>
+      </c>
+      <c r="M2" s="80">
+        <v>1</v>
+      </c>
+      <c r="N2" s="80">
+        <v>0.8</v>
+      </c>
+      <c r="O2" s="80">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="4:60">
       <c r="D3" t="s">
-        <v>127</v>
-      </c>
-      <c r="E3" s="96">
+        <v>126</v>
+      </c>
+      <c r="E3" s="80">
         <v>0.76</v>
       </c>
-      <c r="F3" s="96">
+      <c r="F3" s="80">
         <v>0.92</v>
+      </c>
+      <c r="G3" s="80">
+        <v>0.78</v>
+      </c>
+      <c r="H3" s="80">
+        <v>0.8</v>
+      </c>
+      <c r="I3" s="80">
+        <v>0.78</v>
+      </c>
+      <c r="J3" s="80">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="K3" s="79">
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="L3" s="79">
+        <v>0.83799999999999997</v>
+      </c>
+      <c r="M3" s="80">
+        <v>0.76</v>
+      </c>
+      <c r="N3" s="80">
+        <v>0.78900000000000003</v>
+      </c>
+      <c r="O3" s="80">
+        <v>0.79200000000000004</v>
       </c>
     </row>
     <row r="4" spans="4:60">
       <c r="D4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
         <v>0</v>
+      </c>
+      <c r="G4" s="80">
+        <v>0.2</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="L4" s="80">
+        <v>0.4</v>
       </c>
     </row>
     <row r="6" spans="4:60">
@@ -104453,8 +104523,8 @@
       <c r="I70">
         <v>374</v>
       </c>
-      <c r="J70">
-        <v>0</v>
+      <c r="J70" t="s">
+        <v>129</v>
       </c>
       <c r="K70">
         <v>559</v>

</xml_diff>